<commit_message>
add tomst probe data and script for processing. also deduce photoperiod and max par values for each biweekly timestep
</commit_message>
<xml_diff>
--- a/growth_chamber_progs/TT25_growth_chamber_program_prelim.xlsx
+++ b/growth_chamber_progs/TT25_growth_chamber_program_prelim.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/2025_TT_psf/growth_chamber_progs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23AAB565-0002-9846-9E37-9DA96DF629D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AA79DD2-6F81-7944-AC36-92FE7556CF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4500" yWindow="500" windowWidth="46700" windowHeight="27540" xr2:uid="{67121BAA-B84A-B345-8574-05B08FA4BFC6}"/>
   </bookViews>
@@ -104,10 +104,10 @@
     <t>24-hr time</t>
   </si>
   <si>
-    <t>still need to workshop the exact temp_c and lights_par values and the photoperiod, but the number of steps in the ramp sequence should not change that much. For the canopy closure, we'd really just need to gradually reduce the par over the course of a few days (canopy leaf out takes place over three-five days), so the number of steps in the ramp up/down from daytime to nighttime wouldn't change</t>
-  </si>
-  <si>
     <t>rest of experiment</t>
+  </si>
+  <si>
+    <t>still need to workshop the exact temp_c and lights_par values and the photoperiod, but the number of steps in the ramp sequence should not change that much. For the canopy closure, we'd really just need to gradually reduce the par over the course of a few days (canopy leaf out takes place over ~1 week), so the number of steps in the ramp up/down from daytime to nighttime wouldn't change</t>
   </si>
 </sst>
 </file>
@@ -240,36 +240,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -623,36 +623,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="4">
@@ -667,16 +667,16 @@
       <c r="F2" s="5">
         <v>35</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="2">
         <v>0.45833333333333331</v>
       </c>
@@ -689,12 +689,12 @@
       <c r="F3" s="3">
         <v>70</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4">
         <v>0.875</v>
       </c>
@@ -707,12 +707,12 @@
       <c r="F4" s="5">
         <v>35</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="15"/>
       <c r="C5" s="2">
         <v>0.91666666666666663</v>
       </c>
@@ -725,14 +725,14 @@
       <c r="F5" s="3">
         <v>0</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4">
@@ -747,16 +747,16 @@
       <c r="F6" s="5">
         <v>125</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>22</v>
+      <c r="H6" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="2">
         <v>0.4375</v>
       </c>
@@ -769,12 +769,12 @@
       <c r="F7" s="3">
         <v>250</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="4">
         <v>0.45833333333333331</v>
       </c>
@@ -787,12 +787,12 @@
       <c r="F8" s="5">
         <v>500</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="2">
         <v>0.95833333333333337</v>
       </c>
@@ -805,12 +805,12 @@
       <c r="F9" s="3">
         <v>250</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="4">
         <v>0.97916666666666663</v>
       </c>
@@ -823,12 +823,12 @@
       <c r="F10" s="5">
         <v>125</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="2">
         <v>0</v>
       </c>
@@ -841,15 +841,15 @@
       <c r="F11" s="3">
         <v>0</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>23</v>
+      <c r="B12" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="4">
         <v>0.41666666666666669</v>
@@ -863,14 +863,14 @@
       <c r="F12" s="5">
         <v>200</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="2">
         <v>0.4375</v>
       </c>
@@ -883,12 +883,12 @@
       <c r="F13" s="3">
         <v>400</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="4">
         <v>0.45833333333333331</v>
       </c>
@@ -901,12 +901,12 @@
       <c r="F14" s="5">
         <v>800</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="2">
         <v>0</v>
       </c>
@@ -919,12 +919,12 @@
       <c r="F15" s="3">
         <v>400</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="4">
         <v>2.0833333333333332E-2</v>
       </c>
@@ -937,12 +937,12 @@
       <c r="F16" s="5">
         <v>200</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -955,61 +955,66 @@
       <c r="F17" s="3">
         <v>0</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="H2:H5"/>
+    <mergeCell ref="H6:H17"/>
+    <mergeCell ref="G2:G5"/>
+    <mergeCell ref="G6:G11"/>
+    <mergeCell ref="G12:G17"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B21:D21"/>
@@ -1020,11 +1025,6 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B12:B17"/>
     <mergeCell ref="B6:B11"/>
-    <mergeCell ref="H2:H5"/>
-    <mergeCell ref="H6:H17"/>
-    <mergeCell ref="G2:G5"/>
-    <mergeCell ref="G6:G11"/>
-    <mergeCell ref="G12:G17"/>
     <mergeCell ref="B2:B5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>